<commit_message>
working on the next lab
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\workspace\teaching-bigdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC10C775-D6BD-4781-97DC-B3CB4DC59BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1304E79E-3AA6-4D78-91AE-715D226642ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2565" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Lab</t>
   </si>
@@ -157,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +176,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -195,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,9 +197,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -215,9 +206,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,14 +221,21 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +539,8 @@
     <col min="4" max="4" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="11"/>
+    <col min="7" max="7" width="9.140625" style="9"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -566,7 +562,7 @@
       <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -574,17 +570,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>44860</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <f>WEEKDAY(A2)-1</f>
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1">
@@ -593,86 +589,86 @@
       <c r="F2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="12">
-        <f>SUM($E$2:E2)/$E$15</f>
+      <c r="G2" s="10">
+        <f>SUM($E$2:E2)/$E$17</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>44860</v>
       </c>
-      <c r="B3" s="4">
-        <f t="shared" ref="B3:B14" si="0">WEEKDAY(A3)-1</f>
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="3">
+        <f t="shared" ref="B3:B16" si="0">WEEKDAY(A3)-1</f>
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="12">
-        <f>SUM($E$2:E3)/$E$15</f>
+      <c r="G3" s="10">
+        <f>SUM($E$2:E3)/$E$17</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>44867</v>
       </c>
-      <c r="B4" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="12">
-        <f>SUM($E$2:E4)/$E$15</f>
+      <c r="G4" s="10">
+        <f>SUM($E$2:E4)/$E$17</f>
         <v>0.2</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>44867</v>
       </c>
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="12">
-        <f>SUM($E$2:E5)/$E$15</f>
+      <c r="G5" s="10">
+        <f>SUM($E$2:E5)/$E$17</f>
         <v>0.26666666666666666</v>
       </c>
       <c r="H5" s="1">
@@ -680,53 +676,53 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>44874</v>
       </c>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="12">
-        <f>SUM($E$2:E6)/$E$15</f>
+      <c r="G6" s="10">
+        <f>SUM($E$2:E6)/$E$17</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>44874</v>
       </c>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="12">
-        <f>SUM($E$2:E7)/$E$15</f>
+      <c r="G7" s="10">
+        <f>SUM($E$2:E7)/$E$17</f>
         <v>0.4</v>
       </c>
       <c r="H7" s="1">
@@ -734,53 +730,53 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>44881</v>
       </c>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="12">
-        <f>SUM($E$2:E8)/$E$15</f>
+      <c r="G8" s="10">
+        <f>SUM($E$2:E8)/$E$17</f>
         <v>0.46666666666666667</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>44881</v>
       </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="12">
-        <f>SUM($E$2:E9)/$E$15</f>
+      <c r="G9" s="10">
+        <f>SUM($E$2:E9)/$E$17</f>
         <v>0.53333333333333333</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -788,147 +784,197 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
+        <v>44888</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44888</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>44893</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="11">
-        <f>SUM($E$2:E10)/$E$15</f>
+      <c r="G12" s="10">
+        <f>SUM($E$2:E12)/$E$17</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>44895</v>
       </c>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="11">
-        <f>SUM($E$2:E11)/$E$15</f>
+      <c r="G13" s="9">
+        <f>SUM($E$2:E13)/$E$17</f>
         <v>0.73333333333333328</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H13" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>44895</v>
       </c>
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="11">
-        <f>SUM($E$2:E12)/$E$15</f>
+      <c r="G14" s="9">
+        <f>SUM($E$2:E14)/$E$17</f>
         <v>0.73333333333333328</v>
       </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>44900</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E15" s="1">
         <v>4</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="11">
-        <f>SUM($E$2:E13)/$E$15</f>
+      <c r="G15" s="9">
+        <f>SUM($E$2:E15)/$E$17</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>44907</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="11">
-        <f>SUM($E$2:E14)/$E$15</f>
+      <c r="G16" s="9">
+        <f>SUM($E$2:E16)/$E$17</f>
         <v>1</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="2">
-        <f>SUM(E2:E14)</f>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2">
+        <f>SUM(E2:E16)</f>
         <v>30</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -954,5 +1000,8 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G3:G8" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>